<commit_message>
Chose Which Address to Run
</commit_message>
<xml_diff>
--- a/enderecos.xlsx
+++ b/enderecos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danilo\Desktop\ORGANIZADOR\CODING\PYTHON\FIVERR_IFOOD_SCRAPER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9393930C-A367-4D3F-86FC-178537C61F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A0EC59-BADD-4513-B62E-0DF8C5C2FFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ENDERECOS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ENDERECOS!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ENDERECOS!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Avenida Joao XXIII Saraiva</t>
   </si>
@@ -45,13 +45,19 @@
     <t>NUMERO_DE_PAGINAS</t>
   </si>
   <si>
-    <t>Pirenópolis</t>
-  </si>
-  <si>
     <t>s/n</t>
   </si>
   <si>
     <t>todas</t>
+  </si>
+  <si>
+    <t>COLETAR</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Pirenópolis rua</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -402,7 +408,7 @@
     <col min="3" max="3" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -412,42 +418,54 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>438</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>